<commit_message>
ajust recodedBy, taxon names, site names
</commit_message>
<xml_diff>
--- a/Data/occ_Francini_temporal_abrolhos/Checking.xlsx
+++ b/Data/occ_Francini_temporal_abrolhos/Checking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a9a12216838198/reefsyn_site/Data/occ_Francini_temporal_abrolhos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\ReefSYN_data\Data\occ_Francini_temporal_abrolhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_AD4D361C20488DEA4E38A0DC0CDB46605BDEDD7C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F7D4E0-5E10-466A-B799-64679CB493CB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12844076-1C28-4980-B116-D2423EE61FEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="397">
   <si>
     <t>ABUSAX</t>
   </si>
@@ -1202,6 +1202,24 @@
   </si>
   <si>
     <t>Daniel Santor</t>
+  </si>
+  <si>
+    <t>Ronaldo Francini-Filho</t>
+  </si>
+  <si>
+    <t>Cos(unidentified)</t>
+  </si>
+  <si>
+    <t>No(unidentified)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Mar(unidentified)</t>
+  </si>
+  <si>
+    <t>Dem(unidentified)</t>
   </si>
 </sst>
 </file>
@@ -3026,8 +3044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FE9AAF-64E9-439D-A9B9-2BC893054521}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,6 +3265,9 @@
       <c r="B17" t="s">
         <v>146</v>
       </c>
+      <c r="C17" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -3289,7 +3310,7 @@
         <v>150</v>
       </c>
       <c r="C21" t="s">
-        <v>363</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3332,6 +3353,9 @@
       <c r="B25" t="s">
         <v>154</v>
       </c>
+      <c r="C25" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -3362,6 +3386,9 @@
       <c r="B28" t="s">
         <v>157</v>
       </c>
+      <c r="C28" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -3371,7 +3398,7 @@
         <v>158</v>
       </c>
       <c r="C29" t="s">
-        <v>363</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3426,7 +3453,7 @@
         <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>363</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3447,6 +3474,9 @@
       <c r="B36" t="s">
         <v>164</v>
       </c>
+      <c r="C36" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
@@ -3476,6 +3506,9 @@
       </c>
       <c r="B39" t="s">
         <v>167</v>
+      </c>
+      <c r="C39" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>